<commit_message>
icons on each button vers2
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheetFiles/Internet.xlsx
+++ b/src/main/resources/spreadsheetFiles/Internet.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="fieldnames" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="URL" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="color" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="comments" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="icons" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="48">
   <si>
     <t xml:space="preserve">Internet miscellaneous</t>
   </si>
@@ -124,25 +125,7 @@
     <t xml:space="preserve">https://www.kaggle.com/</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">https://q</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">uickref.me</t>
-    </r>
+    <t xml:space="preserve">https://quickref.me</t>
   </si>
   <si>
     <t xml:space="preserve">https://ourworldindata.org/</t>
@@ -173,6 +156,18 @@
   </si>
   <si>
     <t xml:space="preserve">github !</t>
+  </si>
+  <si>
+    <t xml:space="preserve">globe.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BCN_Logo3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info-circle.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info-circle_red.png</t>
   </si>
 </sst>
 </file>
@@ -183,7 +178,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -220,12 +215,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -272,7 +261,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -302,10 +291,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -394,7 +379,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -525,8 +510,8 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -602,7 +587,7 @@
       <c r="B6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D6" s="3"/>
@@ -650,7 +635,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -716,14 +701,14 @@
       <c r="D5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="9"/>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="6" t="s">
@@ -762,7 +747,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -813,4 +798,101 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:D9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.84"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
WORKING: Final version before code-cleanup
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheetFiles/Internet.xlsx
+++ b/src/main/resources/spreadsheetFiles/Internet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="fieldnames" sheetId="1" state="visible" r:id="rId2"/>
@@ -161,7 +161,7 @@
     <t xml:space="preserve">globe.png</t>
   </si>
   <si>
-    <t xml:space="preserve">BCN_Logo3.png</t>
+    <t xml:space="preserve">BCN_Logo.png</t>
   </si>
   <si>
     <t xml:space="preserve">info-circle.png</t>
@@ -261,7 +261,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -288,6 +288,14 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -378,12 +386,13 @@
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.93"/>
   </cols>
   <sheetData>
@@ -523,98 +532,98 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="9"/>
+      <c r="B5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
-      <c r="C8" s="7" t="s">
+      <c r="A8" s="8"/>
+      <c r="C8" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3"/>
-      <c r="C9" s="3" t="s">
+      <c r="A9" s="8"/>
+      <c r="C9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -701,14 +710,14 @@
       <c r="D5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="8"/>
+      <c r="D6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="6" t="s">
@@ -758,16 +767,16 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -775,12 +784,12 @@
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="9" t="s">
         <v>42</v>
       </c>
     </row>
@@ -807,8 +816,8 @@
   </sheetPr>
   <dimension ref="A2:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
WORKING: clean-up of code
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheetFiles/Internet.xlsx
+++ b/src/main/resources/spreadsheetFiles/Internet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="fieldnames" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,12 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="48">
-  <si>
-    <t xml:space="preserve">Internet miscellaneous</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bioinfo</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="48">
+  <si>
+    <t xml:space="preserve">Internet (miscellaneous)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bioinformatics</t>
   </si>
   <si>
     <t xml:space="preserve">Programming</t>
@@ -261,7 +261,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -288,14 +288,6 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -386,13 +378,13 @@
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.93"/>
   </cols>
   <sheetData>
@@ -520,7 +512,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -532,98 +524,98 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="8"/>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9"/>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="8"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="8"/>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="8"/>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8"/>
-      <c r="C8" s="9" t="s">
+      <c r="A8" s="3"/>
+      <c r="C8" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8"/>
-      <c r="C9" s="8" t="s">
+      <c r="A9" s="3"/>
+      <c r="C9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -710,14 +702,14 @@
       <c r="D5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="6" t="s">
@@ -756,7 +748,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -767,16 +759,16 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -784,12 +776,12 @@
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -814,10 +806,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:D9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -828,6 +820,20 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.84"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>44</v>

</xml_diff>